<commit_message>
Update Plan de Trabajo Cristhian.xlsx
</commit_message>
<xml_diff>
--- a/Entregables/Cristhian/Plan de Trabajo Cristhian.xlsx
+++ b/Entregables/Cristhian/Plan de Trabajo Cristhian.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="27870" windowHeight="14310"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="27870" windowHeight="14310"/>
   </bookViews>
   <sheets>
     <sheet name="PLAN DE TRABAJO" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>Producto</t>
   </si>
@@ -160,12 +160,6 @@
   </si>
   <si>
     <t>Envió de correo electrónico con el plan de trabajo y los documentos de análisis y planeación</t>
-  </si>
-  <si>
-    <t>Código fuente</t>
-  </si>
-  <si>
-    <t>Elaborar documentación solicitada</t>
   </si>
   <si>
     <t>Participar en reuniones técnicas con el equipo de control y seguimiento y funcionales encargados de la Dirección de reparación</t>
@@ -200,6 +194,19 @@
   <si>
     <t>Desarrollo en Maariv de:
 - FICHA DE DOCUMENTO DE FORMULACIÓN PLAN ELABORADA POR EL SISTEMA</t>
+  </si>
+  <si>
+    <t>Informe de avance</t>
+  </si>
+  <si>
+    <t>Código fuente y acta de aceptación</t>
+  </si>
+  <si>
+    <t>Elaborar documentación solicitada
+- Manual de usuario
+- Manual de administración
+- Diagrama de clases
+- Diagram de componentes</t>
   </si>
 </sst>
 </file>
@@ -431,12 +438,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -448,6 +449,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -788,7 +795,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -822,43 +829,43 @@
       <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15" t="s">
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
       <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14" t="s">
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
     </row>
     <row r="3" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="22"/>
@@ -900,14 +907,14 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="18">
+      <c r="A4" s="16">
         <v>1</v>
       </c>
       <c r="B4" s="25" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>31</v>
@@ -925,8 +932,8 @@
       <c r="O4" s="7"/>
     </row>
     <row r="5" spans="1:15" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="17"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="5" t="s">
         <v>25</v>
       </c>
@@ -946,8 +953,8 @@
       <c r="O5" s="7"/>
     </row>
     <row r="6" spans="1:15" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="16" t="s">
+      <c r="A6" s="16"/>
+      <c r="B6" s="14" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -969,10 +976,10 @@
       <c r="O6" s="7"/>
     </row>
     <row r="7" spans="1:15" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="17"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>33</v>
@@ -990,7 +997,7 @@
       <c r="O7" s="7"/>
     </row>
     <row r="8" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="9" t="s">
         <v>26</v>
       </c>
@@ -1013,7 +1020,7 @@
       <c r="O8" s="11"/>
     </row>
     <row r="9" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="18">
+      <c r="A9" s="16">
         <v>2</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -1023,7 +1030,7 @@
         <v>35</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="6"/>
@@ -1038,15 +1045,15 @@
       <c r="O9" s="7"/>
     </row>
     <row r="10" spans="1:15" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="16" t="s">
+      <c r="A10" s="16"/>
+      <c r="B10" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>47</v>
-      </c>
       <c r="D10" s="5" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="7"/>
@@ -1061,13 +1068,13 @@
       <c r="O10" s="7"/>
     </row>
     <row r="11" spans="1:15" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="17"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="7"/>
@@ -1082,7 +1089,7 @@
       <c r="O11" s="7"/>
     </row>
     <row r="12" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
+      <c r="A12" s="17"/>
       <c r="B12" s="9" t="s">
         <v>28</v>
       </c>
@@ -1105,7 +1112,7 @@
       <c r="O12" s="11"/>
     </row>
     <row r="13" spans="1:15" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="18">
+      <c r="A13" s="16">
         <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -1130,15 +1137,15 @@
       <c r="O13" s="7"/>
     </row>
     <row r="14" spans="1:15" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="16" t="s">
-        <v>46</v>
+      <c r="A14" s="16"/>
+      <c r="B14" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="7"/>
@@ -1153,13 +1160,13 @@
       <c r="O14" s="6"/>
     </row>
     <row r="15" spans="1:15" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="17"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="15"/>
       <c r="C15" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="7"/>
@@ -1174,12 +1181,12 @@
       <c r="O15" s="6"/>
     </row>
     <row r="16" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="9" t="s">
         <v>30</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>39</v>
@@ -1198,11 +1205,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="F2:J2"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="F1:J1"/>
     <mergeCell ref="B6:B7"/>
@@ -1213,6 +1215,11 @@
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="D1:D3"/>
     <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="F2:J2"/>
   </mergeCells>
   <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="0.74803149606299213" bottom="0.51181102362204722" header="0.51181102362204722" footer="0.74803149606299213"/>
   <pageSetup scale="58" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>